<commit_message>
added Dexibuprofen to NSAIDs set
</commit_message>
<xml_diff>
--- a/protected/data/dmd_data/Drug-Type-Mappings.xlsx
+++ b/protected/data/dmd_data/Drug-Type-Mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c58bff20204d3898/Documents/docker-compose/MM/dmd_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="11_611EE3B2B6AEC4E91FAFF6C24585CFD48B53695D" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1884293B-2C79-480C-ACA6-99C33C7B34BC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FB4C39-CB1B-4738-8345-8352C39E7565}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="750" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15330" tabRatio="750" firstSheet="19" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Non-opioid Analgesic" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="788">
   <si>
     <t>Term</t>
   </si>
@@ -2428,6 +2428,12 @@
   </si>
   <si>
     <t>Simple Analgesics</t>
+  </si>
+  <si>
+    <t>Dexibuprofen</t>
+  </si>
+  <si>
+    <t>418027007</t>
   </si>
 </sst>
 </file>
@@ -8120,10 +8126,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <dimension ref="A1:AMK12"/>
+  <dimension ref="A1:AMK13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8262,6 +8268,17 @@
         <v>570</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -9087,7 +9104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add some additional Penecillin allergy mappings
</commit_message>
<xml_diff>
--- a/protected/data/dmd_data/Drug-Type-Mappings.xlsx
+++ b/protected/data/dmd_data/Drug-Type-Mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FB4C39-CB1B-4738-8345-8352C39E7565}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5DDBFA-26F1-42B8-A601-8347BF664499}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15330" tabRatio="750" firstSheet="19" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="750" firstSheet="30" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Non-opioid Analgesic" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="790">
   <si>
     <t>Term</t>
   </si>
@@ -2434,6 +2434,12 @@
   </si>
   <si>
     <t>418027007</t>
+  </si>
+  <si>
+    <t>89519005</t>
+  </si>
+  <si>
+    <t>96067005</t>
   </si>
 </sst>
 </file>
@@ -8128,7 +8134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:AMK13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -10643,10 +10649,10 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10731,6 +10737,28 @@
         <v>765</v>
       </c>
       <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="C9" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>